<commit_message>
modify test cases of mysql
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/databrain-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/databrain-connector-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC20347-3C52-4014-B72D-63CDA1B2D67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A704AF01-79D7-445A-8A3D-FAFAF55B82D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>runningTime</t>
+  </si>
+  <si>
+    <t>clickhouseJdbcUrl</t>
+  </si>
+  <si>
+    <t>jdbc:clickhouse://140.231.89.85:30642</t>
   </si>
 </sst>
 </file>
@@ -540,9 +546,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ABFD6B-5C24-4B5A-830A-CA8DC1E4BA91}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -606,10 +612,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3518E73-3678-49EC-A844-38B9E4DC824C}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -617,14 +623,16 @@
     <col min="1" max="1" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="12.6640625" style="1"/>
+    <col min="4" max="4" width="32.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -635,19 +643,25 @@
         <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>15</v>
       </c>
@@ -658,11 +672,17 @@
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3">
+        <v>10</v>
+      </c>
       <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add test cases for data-brain-test
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/databrain-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/databrain-connector-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-backup\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2D6CA06-968D-4D29-A58F-FEEB6F45F636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E74C3DE-C7ED-45C2-8FB4-913C20F7BAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="834" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
   <si>
     <t>name</t>
   </si>
@@ -142,9 +142,6 @@
   </si>
   <si>
     <t>databrain-getConceptModelDataByCondition-test-2</t>
-  </si>
-  <si>
-    <t>good request, data retrieved(no schema check)</t>
   </si>
   <si>
     <t>sensor</t>
@@ -199,36 +196,74 @@
   <si>
     <t>isObj</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>good request, data retrieved(no schema check)
+read desigoCC history data</t>
+  </si>
+  <si>
+    <t>good request, data retrieved(no schema check)
+read desigoCC realtime data</t>
+  </si>
+  <si>
+    <t>good request, data retrieved(no schema check)
+read enlighted history data</t>
+  </si>
+  <si>
+    <t>SubscriptionValue</t>
+  </si>
+  <si>
+    <t>good request, data retrieved(no schema check)
+read MQTT realtime data</t>
+  </si>
+  <si>
+    <t>databrain-getConceptModelDataByCondition-test-3</t>
+  </si>
+  <si>
+    <t>databrain-getConceptModelDataByCondition-test-4</t>
+  </si>
+  <si>
+    <t>databrain-getConceptModelDataByCondition-test-5</t>
+  </si>
+  <si>
+    <t>databrain-getConceptModelDataByCondition-test-6</t>
+  </si>
+  <si>
+    <t>databrain-getConceptModelDataByCondition-test-7</t>
+  </si>
+  <si>
+    <t>good request, data retrieved(no schema check)
+read desigoCC realtime data/case for SDL-6773</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -275,14 +310,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,112 +607,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78214A11-4EBC-4BA5-ABD2-BD145C64902F}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="41.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="12.6640625" style="1"/>
+    <col min="1" max="1" width="32.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.77734375" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="12.6640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:13" ht="41.4">
+      <c r="A2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="B2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="1:13" ht="41.4">
+      <c r="A3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6">
+        <v>10</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="1:13" ht="41.4">
+      <c r="A4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:13" ht="41.4">
+      <c r="A5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+    </row>
+    <row r="6" spans="1:13" ht="41.4">
+      <c r="A6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:13" ht="41.4">
+      <c r="A7" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:13" ht="41.4">
+      <c r="A8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6">
+        <v>10</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -683,10 +842,10 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="30.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -699,7 +858,7 @@
     <col min="9" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -725,7 +884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -757,10 +916,10 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="32" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -774,7 +933,7 @@
     <col min="10" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -803,7 +962,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -835,30 +994,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DBFB8D-492D-4320-9CD5-02DB7169B8BB}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="34.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="31.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" style="1" customWidth="1"/>
-    <col min="6" max="7" width="13.109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="78.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="33.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="60.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -875,10 +1034,10 @@
         <v>32</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>31</v>
@@ -899,21 +1058,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -928,7 +1087,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -953,57 +1112,63 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="3">
         <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" s="6" t="s">
+      <c r="F5" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D7" s="6"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D9" s="6"/>
+      <c r="G5" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
update test case which pass well
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/databrain-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/databrain-connector-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-backup\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E74C3DE-C7ED-45C2-8FB4-913C20F7BAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5E941A-1854-4287-99CE-5AD04F4CAE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-14570" windowWidth="38620" windowHeight="21220" tabRatio="834" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
   <si>
     <t>name</t>
   </si>
@@ -163,23 +163,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>202201051000</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>202201051005</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>databrain-enlightedHistoryData-test-4</t>
-  </si>
-  <si>
-    <t>202201111500</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>202201111600</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>sensor_id</t>
@@ -234,36 +218,48 @@
   <si>
     <t>good request, data retrieved(no schema check)
 read desigoCC realtime data/case for SDL-6773</t>
+  </si>
+  <si>
+    <t>202203071530</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>202203071537</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>202203071540</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -609,11 +605,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78214A11-4EBC-4BA5-ABD2-BD145C64902F}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.44140625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" style="8" bestFit="1" customWidth="1"/>
@@ -631,7 +627,7 @@
     <col min="14" max="16384" width="12.6640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
@@ -672,12 +668,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="41.4">
+    <row r="2" spans="1:13" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>23</v>
@@ -695,12 +691,12 @@
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
     </row>
-    <row r="3" spans="1:13" ht="41.4">
+    <row r="3" spans="1:13" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -718,12 +714,12 @@
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
     </row>
-    <row r="4" spans="1:13" ht="41.4">
+    <row r="4" spans="1:13" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>24</v>
@@ -741,12 +737,12 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
     </row>
-    <row r="5" spans="1:13" ht="41.4">
+    <row r="5" spans="1:13" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>22</v>
@@ -764,12 +760,12 @@
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
     </row>
-    <row r="6" spans="1:13" ht="41.4">
+    <row r="6" spans="1:13" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -785,12 +781,12 @@
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
     </row>
-    <row r="7" spans="1:13" ht="41.4">
+    <row r="7" spans="1:13" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -806,18 +802,18 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
     </row>
-    <row r="8" spans="1:13" ht="41.4">
+    <row r="8" spans="1:13" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -845,7 +841,7 @@
       <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -858,7 +854,7 @@
     <col min="9" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -884,7 +880,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -919,7 +915,7 @@
       <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -933,7 +929,7 @@
     <col min="10" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -962,7 +958,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
@@ -996,16 +992,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DBFB8D-492D-4320-9CD5-02DB7169B8BB}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -1017,7 +1014,7 @@
     <col min="14" max="16384" width="12.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -1037,7 +1034,7 @@
         <v>38</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>31</v>
@@ -1058,7 +1055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1087,7 +1084,7 @@
       <c r="L2" s="3"/>
       <c r="M2" s="3"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
@@ -1112,7 +1109,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>39</v>
       </c>
@@ -1123,16 +1120,16 @@
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>44</v>
+        <v>59</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -1141,9 +1138,9 @@
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
@@ -1152,16 +1149,16 @@
         <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="G5" s="9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>

</xml_diff>

<commit_message>
add test cases of SDL-6799
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/databrain-connector-test-data.xlsx
+++ b/src/main/resources/test-data-xls/databrain-connector-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E74C3DE-C7ED-45C2-8FB4-913C20F7BAE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EBEA22F-C9E0-4571-9153-9804B6AB3370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="834" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="getConceptModelDataByCondition" sheetId="3" r:id="rId1"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78214A11-4EBC-4BA5-ABD2-BD145C64902F}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>
@@ -996,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35DBFB8D-492D-4320-9CD5-02DB7169B8BB}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="13.8"/>

</xml_diff>